<commit_message>
please upload this time
</commit_message>
<xml_diff>
--- a/washingtondczipsandneighborhoods.xlsx
+++ b/washingtondczipsandneighborhoods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pcori-my.sharepoint.com/personal/rbloodworth_pcori_org/Documents/Misc/githubprojects/Coursera_Capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{5102244E-8C80-4C79-AF7E-FCCC7E78DEDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5A2B58A-9D2E-4244-8477-83CE8D666E1F}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{5102244E-8C80-4C79-AF7E-FCCC7E78DEDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82D2CFFA-DE6F-4DF5-ABD3-E69EDC6C9D6C}"/>
   <bookViews>
     <workbookView xWindow="10140" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{D75602E0-7E9D-4507-B259-0FDC3D72C17A}"/>
   </bookViews>
@@ -592,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B21CDC5-4E91-43F2-87B0-B2205AFCEC0E}">
   <dimension ref="A1:A131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67:A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,6 +927,12 @@
       <c r="A66" s="1" t="s">
         <v>65</v>
       </c>
+    </row>
+    <row r="67" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="1"/>
+    </row>
+    <row r="68" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="1"/>
     </row>
     <row r="131" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>

</xml_diff>

<commit_message>
trying to add just one file...
</commit_message>
<xml_diff>
--- a/washingtondczipsandneighborhoods.xlsx
+++ b/washingtondczipsandneighborhoods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pcori-my.sharepoint.com/personal/rbloodworth_pcori_org/Documents/Misc/githubprojects/Coursera_Capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{5102244E-8C80-4C79-AF7E-FCCC7E78DEDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82D2CFFA-DE6F-4DF5-ABD3-E69EDC6C9D6C}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{5102244E-8C80-4C79-AF7E-FCCC7E78DEDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4B9DC9F-5EA9-4D45-B79F-0CF8A3BBB886}"/>
   <bookViews>
     <workbookView xWindow="10140" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{D75602E0-7E9D-4507-B259-0FDC3D72C17A}"/>
   </bookViews>
@@ -593,7 +593,7 @@
   <dimension ref="A1:A131"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67:A68"/>
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>